<commit_message>
menambahkan fungsi bulk toko csv
</commit_message>
<xml_diff>
--- a/Outlet_TDN_Eksisting.xlsx
+++ b/Outlet_TDN_Eksisting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\it_de\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/web/SnjMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D718172-FE5D-4EBF-ADA4-6C043FCDA350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BE24CC-102F-404D-9CEB-54045248C841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="125">
   <si>
     <t>No</t>
   </si>
@@ -386,6 +386,15 @@
   </si>
   <si>
     <t>https://mapidstorage.s3.ap-southeast-1.amazonaws.com/general_image/kingkinmhr/1767622608519_img_%25Toko%20Daging%20Nusantara_%254a532228-5a74-4760-ae5f-a6e25c0faca6.png</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>on-Survey</t>
   </si>
 </sst>
 </file>
@@ -745,46 +754,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.125" customWidth="1"/>
-    <col min="4" max="4" width="35.625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -792,22 +805,25 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>-6.4205825101226397</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>107.47344356796</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -815,22 +831,25 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-7.0027013519730996</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>107.55252837671701</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -838,22 +857,25 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>-7.4383469126930697</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>109.24410918255499</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -861,22 +883,25 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>-6.3087709832655001</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>106.889097531147</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -884,22 +909,25 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>-6.2599305395101998</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>106.80792982134101</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -907,22 +935,25 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>-6.9891450268730901</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>110.448043922826</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -930,22 +961,25 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>-6.2617525038157504</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>107.143208923267</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -953,22 +987,25 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>37</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>-6.1826839202877197</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>106.719335318939</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -976,22 +1013,25 @@
         <v>39</v>
       </c>
       <c r="C10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>-6.1825906374774604</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>106.626522339853</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -999,22 +1039,25 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>-6.1916652962268097</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>106.84763859253</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1022,22 +1065,25 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>49</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>-6.2307632645998003</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>106.846221395611</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1045,22 +1091,25 @@
         <v>51</v>
       </c>
       <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>53</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>-6.1876455242893362</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>106.898844254202</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1068,22 +1117,25 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>57</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>-6.2326294666362072</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>106.974442429321</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1091,22 +1143,25 @@
         <v>59</v>
       </c>
       <c r="C15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>61</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>-6.4115158789179221</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>106.819553764264</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1114,22 +1169,25 @@
         <v>63</v>
       </c>
       <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
         <v>64</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>65</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>-6.351402080432738</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>106.921627917072</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1137,22 +1195,25 @@
         <v>67</v>
       </c>
       <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>69</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>-6.5704349011957763</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>106.75644654782459</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1160,22 +1221,25 @@
         <v>71</v>
       </c>
       <c r="C18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" t="s">
         <v>72</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>73</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>-6.4725036608022402</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>106.820574526982</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1183,22 +1247,25 @@
         <v>75</v>
       </c>
       <c r="C19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>76</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>-6.41043747232243</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>106.961465857672</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1206,22 +1273,25 @@
         <v>78</v>
       </c>
       <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" t="s">
         <v>79</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>80</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>-6.2532270318058822</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>106.68577506900498</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1229,22 +1299,25 @@
         <v>82</v>
       </c>
       <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>84</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>-6.4367452551869695</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>106.80818262883584</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1252,22 +1325,25 @@
         <v>86</v>
       </c>
       <c r="C22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>88</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>-6.2084093103080589</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>106.9365578753588</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1275,22 +1351,25 @@
         <v>90</v>
       </c>
       <c r="C23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>92</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>-5.1079730203704603</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>119.5109164576717</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1298,22 +1377,25 @@
         <v>94</v>
       </c>
       <c r="C24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" t="s">
         <v>95</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>96</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>-6.1734849146599666</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>106.68485740737593</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1321,22 +1403,25 @@
         <v>98</v>
       </c>
       <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" t="s">
         <v>99</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>100</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>-6.2460925552455731</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>107.01056506187057</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1344,22 +1429,25 @@
         <v>102</v>
       </c>
       <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" t="s">
         <v>103</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>104</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>-6.2463609072791773</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>107.06155664439133</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1367,22 +1455,25 @@
         <v>106</v>
       </c>
       <c r="C27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" t="s">
         <v>107</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>108</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>-6.3202204638651667</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>106.82537817116413</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1390,22 +1481,25 @@
         <v>110</v>
       </c>
       <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>112</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>-6.2925682593457797</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>106.73271037116415</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1413,22 +1507,25 @@
         <v>114</v>
       </c>
       <c r="C29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>116</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>-6.2935384373811374</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>106.81637675398302</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1436,18 +1533,21 @@
         <v>118</v>
       </c>
       <c r="C30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
         <v>119</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>120</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>-6.1826470004907526</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>106.78357672853592</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>